<commit_message>
Update column names: Clarify snow depth measurement
- Changed "Sne" to "Snedybde" (snow depth) in column names
- Updated all table headers and data labels
- Changed summary card to "Gns. Snedybdeforskel"
- Makes it clear we measure depth not snowfall

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/weather_impact_interactive.xlsx
+++ b/weather_impact_interactive.xlsx
@@ -428,10 +428,10 @@
         <v>Nedbør 2025</v>
       </c>
       <c r="I1" t="str">
-        <v>Sne 2026</v>
+        <v>Snedybde 2026 (cm)</v>
       </c>
       <c r="J1" t="str">
-        <v>Sne 2025</v>
+        <v>Snedybde 2025 (cm)</v>
       </c>
       <c r="K1" t="str">
         <v>Impact</v>

</xml_diff>